<commit_message>
Added partial functionality for memory ops
</commit_message>
<xml_diff>
--- a/Project Status.xlsx
+++ b/Project Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\Sheffield\Dissertation\Implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCD2FBB-6273-4251-B24E-A5523F0E54D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C01E37-3DA8-464D-8A36-38D5D343F065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{6AEECA0D-8F2C-4A55-83E2-29C119C2CE7B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
   <si>
     <t>Class Name</t>
   </si>
@@ -104,16 +104,25 @@
     <t>Not Started</t>
   </si>
   <si>
-    <t>Dummy Methods</t>
-  </si>
-  <si>
-    <t>Dummy Methods (incorrect)</t>
-  </si>
-  <si>
-    <t>Signed functions need reviewing</t>
-  </si>
-  <si>
     <t>Complete</t>
+  </si>
+  <si>
+    <t>Signed ops need completing</t>
+  </si>
+  <si>
+    <t>Exception Classes</t>
+  </si>
+  <si>
+    <t>FormatBytecode</t>
+  </si>
+  <si>
+    <t>Decoder</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Add a 'Run' class to run sys</t>
   </si>
 </sst>
 </file>
@@ -203,28 +212,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -561,15 +549,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3524D0-160D-4C96-AB93-A63D0D7A8380}">
-  <dimension ref="B3:E16"/>
+  <dimension ref="B3:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="18.47265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.20703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.05078125" bestFit="1" customWidth="1"/>
   </cols>
@@ -597,7 +585,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>16</v>
@@ -610,8 +598,8 @@
       <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>24</v>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>17</v>
@@ -625,7 +613,7 @@
         <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>16</v>
@@ -639,7 +627,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>16</v>
@@ -667,7 +655,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>16</v>
@@ -681,7 +669,7 @@
         <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>16</v>
@@ -695,7 +683,7 @@
         <v>17</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>17</v>
@@ -709,7 +697,7 @@
         <v>19</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>20</v>
@@ -722,7 +710,7 @@
       <c r="C14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -737,7 +725,7 @@
         <v>16</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>17</v>
@@ -757,15 +745,71 @@
         <v>17</v>
       </c>
     </row>
+    <row r="17" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:E16">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Yes">
+  <conditionalFormatting sqref="C5:E20">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",C5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C5)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added exception handling for unimplemented opcodes
</commit_message>
<xml_diff>
--- a/Project Status.xlsx
+++ b/Project Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\Sheffield\Dissertation\Implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C01E37-3DA8-464D-8A36-38D5D343F065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD1D805-34AC-4A57-8B4C-112B2FBEA7C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{6AEECA0D-8F2C-4A55-83E2-29C119C2CE7B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
   <si>
     <t>Class Name</t>
   </si>
@@ -89,9 +89,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Not Working On</t>
-  </si>
-  <si>
     <t>Yes?</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>Currently Working On</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t>Complete</t>
   </si>
   <si>
@@ -123,6 +117,9 @@
   </si>
   <si>
     <t>Add a 'Run' class to run sys</t>
+  </si>
+  <si>
+    <t>Block Operations</t>
   </si>
 </sst>
 </file>
@@ -164,7 +161,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -187,11 +184,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -206,6 +216,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -549,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3524D0-160D-4C96-AB93-A63D0D7A8380}">
-  <dimension ref="B3:E20"/>
+  <dimension ref="B3:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -564,16 +580,16 @@
   <sheetData>
     <row r="3" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="4" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -585,7 +601,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>16</v>
@@ -599,7 +615,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>17</v>
@@ -613,7 +629,7 @@
         <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>16</v>
@@ -627,7 +643,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>16</v>
@@ -638,13 +654,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -655,7 +671,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>16</v>
@@ -669,7 +685,7 @@
         <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>16</v>
@@ -683,49 +699,49 @@
         <v>17</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B13" s="1" t="s">
-        <v>10</v>
+      <c r="B13" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>24</v>
+        <v>11</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>17</v>
@@ -733,12 +749,12 @@
     </row>
     <row r="16" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E16" s="4" t="s">
@@ -746,14 +762,14 @@
       </c>
     </row>
     <row r="17" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>16</v>
@@ -761,13 +777,13 @@
     </row>
     <row r="18" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>16</v>
@@ -775,42 +791,56 @@
     </row>
     <row r="19" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:E20">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C5)))</formula>
+  <conditionalFormatting sqref="C5:E21">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",C5)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",C5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",C5)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improved exception handling, decoder now fully functional
</commit_message>
<xml_diff>
--- a/Project Status.xlsx
+++ b/Project Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\Sheffield\Dissertation\Implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD1D805-34AC-4A57-8B4C-112B2FBEA7C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DC15DF-AABE-414F-A355-C6908A76333B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{6AEECA0D-8F2C-4A55-83E2-29C119C2CE7B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="34">
   <si>
     <t>Class Name</t>
   </si>
@@ -120,6 +120,21 @@
   </si>
   <si>
     <t>Block Operations</t>
+  </si>
+  <si>
+    <t>Write functions for Jump/JumpI</t>
+  </si>
+  <si>
+    <t>Add functions for SelfDestruct/Stop</t>
+  </si>
+  <si>
+    <t>Add functionality to identify function hashes</t>
+  </si>
+  <si>
+    <t>Sort NumberFormatExceptions in arithmetic ops</t>
+  </si>
+  <si>
+    <t>Not Started</t>
   </si>
 </sst>
 </file>
@@ -161,7 +176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -184,24 +199,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -216,12 +218,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -565,31 +561,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3524D0-160D-4C96-AB93-A63D0D7A8380}">
-  <dimension ref="B3:E21"/>
+  <dimension ref="B3:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="21.734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.20703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.05078125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="4" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -696,7 +692,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>21</v>
@@ -831,8 +827,64 @@
         <v>16</v>
       </c>
     </row>
+    <row r="22" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:E21">
+  <conditionalFormatting sqref="C5:E25">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C5)))</formula>
     </cfRule>

</xml_diff>